<commit_message>
Arreglo Datos de proveedor FT. Agrego Robo FT y no FT.
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A42F9C-0BF4-46B3-8991-59D4B5091DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D015938-B74C-405A-80F6-39DA3425FA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="78">
   <si>
     <t>Usuario</t>
   </si>
@@ -234,13 +234,31 @@
     <t>04104018336</t>
   </si>
   <si>
-    <t>04104018434</t>
-  </si>
-  <si>
-    <t>26/05/2021</t>
-  </si>
-  <si>
     <t>Granizo</t>
+  </si>
+  <si>
+    <t>ROBO</t>
+  </si>
+  <si>
+    <t>CodProveedorRobo</t>
+  </si>
+  <si>
+    <t>27433</t>
+  </si>
+  <si>
+    <t>DescripcionRobo</t>
+  </si>
+  <si>
+    <t>Rueda</t>
+  </si>
+  <si>
+    <t>04104018548</t>
+  </si>
+  <si>
+    <t>Batería</t>
+  </si>
+  <si>
+    <t>08/08/2021</t>
   </si>
 </sst>
 </file>
@@ -616,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +657,7 @@
     <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -712,8 +730,17 @@
       <c r="X1" t="s">
         <v>7</v>
       </c>
+      <c r="Y1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -730,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>49</v>
@@ -786,8 +813,11 @@
       <c r="X2" t="s">
         <v>9</v>
       </c>
+      <c r="Y2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -804,13 +834,13 @@
         <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>49</v>
@@ -860,8 +890,11 @@
       <c r="X3" t="s">
         <v>9</v>
       </c>
+      <c r="Y3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -878,13 +911,13 @@
         <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>49</v>
@@ -925,17 +958,24 @@
       <c r="U4" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="V4" s="1"/>
       <c r="W4" t="s">
         <v>8</v>
       </c>
       <c r="X4" t="s">
         <v>9</v>
       </c>
+      <c r="Y4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA4">
+        <v>27433</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -952,13 +992,13 @@
         <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>49</v>
@@ -997,7 +1037,7 @@
         <v>9</v>
       </c>
       <c r="U5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" t="s">
@@ -1006,8 +1046,14 @@
       <c r="X5" t="s">
         <v>9</v>
       </c>
+      <c r="Y5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1077,8 +1123,11 @@
       <c r="X6" t="s">
         <v>9</v>
       </c>
+      <c r="Y6" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1148,8 +1197,11 @@
       <c r="X7" t="s">
         <v>9</v>
       </c>
+      <c r="Y7" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1214,7 +1266,7 @@
         <v>48</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="W8" t="s">
         <v>8</v>
@@ -1222,8 +1274,11 @@
       <c r="X8" t="s">
         <v>9</v>
       </c>
+      <c r="Y8" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1293,8 +1348,11 @@
       <c r="X9" t="s">
         <v>9</v>
       </c>
+      <c r="Y9" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1352,6 +1410,9 @@
       <c r="S10" t="s">
         <v>10</v>
       </c>
+      <c r="T10" t="s">
+        <v>9</v>
+      </c>
       <c r="U10" t="s">
         <v>34</v>
       </c>
@@ -1361,8 +1422,11 @@
       <c r="X10" t="s">
         <v>9</v>
       </c>
+      <c r="Y10" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1420,6 +1484,9 @@
       <c r="S11" t="s">
         <v>10</v>
       </c>
+      <c r="T11" t="s">
+        <v>9</v>
+      </c>
       <c r="U11" t="s">
         <v>34</v>
       </c>
@@ -1429,8 +1496,11 @@
       <c r="X11" t="s">
         <v>9</v>
       </c>
+      <c r="Y11" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1488,6 +1558,9 @@
       <c r="S12" t="s">
         <v>10</v>
       </c>
+      <c r="T12" t="s">
+        <v>9</v>
+      </c>
       <c r="U12" t="s">
         <v>34</v>
       </c>
@@ -1497,8 +1570,11 @@
       <c r="X12" t="s">
         <v>9</v>
       </c>
+      <c r="Y12" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1556,6 +1632,9 @@
       <c r="S13" t="s">
         <v>41</v>
       </c>
+      <c r="T13" t="s">
+        <v>9</v>
+      </c>
       <c r="U13" t="s">
         <v>42</v>
       </c>
@@ -1565,8 +1644,11 @@
       <c r="X13" t="s">
         <v>9</v>
       </c>
+      <c r="Y13" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1639,8 +1721,11 @@
       <c r="X14" t="s">
         <v>9</v>
       </c>
+      <c r="Y14" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1713,8 +1798,11 @@
       <c r="X15" t="s">
         <v>9</v>
       </c>
+      <c r="Y15" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1787,8 +1875,11 @@
       <c r="X16" t="s">
         <v>9</v>
       </c>
+      <c r="Y16" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1859,6 +1950,9 @@
         <v>8</v>
       </c>
       <c r="X17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y17" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
arreglo FT para que acepte FT daños y robo a la vez
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D015938-B74C-405A-80F6-39DA3425FA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA548374-9ED5-4B2A-A1BA-1BD474CAAD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="79">
   <si>
     <t>Usuario</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Motor</t>
   </si>
   <si>
-    <t>04005237931</t>
-  </si>
-  <si>
     <t>04005237932</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>12:30</t>
   </si>
   <si>
-    <t xml:space="preserve">04104016410 </t>
-  </si>
-  <si>
     <t>30/04/2020</t>
   </si>
   <si>
@@ -259,6 +253,15 @@
   </si>
   <si>
     <t>08/08/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04104015957 </t>
+  </si>
+  <si>
+    <t>05/05/2021</t>
+  </si>
+  <si>
+    <t>04104015957</t>
   </si>
 </sst>
 </file>
@@ -341,12 +344,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -636,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,13 +661,13 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -710,19 +712,19 @@
         <v>19</v>
       </c>
       <c r="R1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S1" t="s">
         <v>5</v>
       </c>
       <c r="T1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U1" t="s">
         <v>15</v>
       </c>
       <c r="V1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W1" t="s">
         <v>6</v>
@@ -731,13 +733,13 @@
         <v>7</v>
       </c>
       <c r="Y1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Z1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AA1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -745,10 +747,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -757,25 +759,25 @@
         <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>77</v>
+      <c r="H2" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J2">
         <v>32039201</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>29</v>
+      <c r="K2" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M2" t="s">
         <v>20</v>
@@ -784,28 +786,28 @@
         <v>19</v>
       </c>
       <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>32</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>33</v>
       </c>
       <c r="R2">
         <v>967</v>
       </c>
       <c r="S2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T2" t="s">
         <v>8</v>
       </c>
       <c r="U2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W2" t="s">
         <v>8</v>
@@ -822,10 +824,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -834,25 +836,25 @@
         <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>77</v>
+      <c r="H3" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J3">
         <v>32039201</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>29</v>
+      <c r="K3" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M3" t="s">
         <v>20</v>
@@ -861,28 +863,28 @@
         <v>19</v>
       </c>
       <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" t="s">
         <v>31</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>32</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>33</v>
       </c>
       <c r="R3">
         <v>967</v>
       </c>
       <c r="S3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T3" t="s">
         <v>8</v>
       </c>
       <c r="U3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W3" t="s">
         <v>8</v>
@@ -899,10 +901,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -911,25 +913,25 @@
         <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>77</v>
+      <c r="H4" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4">
         <v>32039201</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>29</v>
+      <c r="K4" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M4" t="s">
         <v>20</v>
@@ -938,25 +940,25 @@
         <v>19</v>
       </c>
       <c r="O4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" t="s">
         <v>31</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>32</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>33</v>
       </c>
       <c r="R4">
         <v>967</v>
       </c>
       <c r="S4" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U4" t="s">
         <v>41</v>
-      </c>
-      <c r="T4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U4" t="s">
-        <v>42</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" t="s">
@@ -969,7 +971,7 @@
         <v>8</v>
       </c>
       <c r="Z4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AA4">
         <v>27433</v>
@@ -980,10 +982,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -992,25 +994,25 @@
         <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>77</v>
+      <c r="H5" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5">
         <v>32039201</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>29</v>
+      <c r="K5" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M5" t="s">
         <v>20</v>
@@ -1019,25 +1021,25 @@
         <v>19</v>
       </c>
       <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" t="s">
         <v>31</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>32</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>33</v>
       </c>
       <c r="R5">
         <v>967</v>
       </c>
       <c r="S5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T5" t="s">
         <v>9</v>
       </c>
       <c r="U5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" t="s">
@@ -1050,7 +1052,7 @@
         <v>8</v>
       </c>
       <c r="Z5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -1058,10 +1060,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -1070,25 +1072,25 @@
         <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>67</v>
+      <c r="H6" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6">
         <v>32039201</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>29</v>
+      <c r="K6" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M6" t="s">
         <v>20</v>
@@ -1097,25 +1099,28 @@
         <v>19</v>
       </c>
       <c r="O6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" t="s">
         <v>31</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>32</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>33</v>
       </c>
       <c r="R6">
         <v>967</v>
       </c>
       <c r="S6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U6" t="s">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="W6" t="s">
         <v>8</v>
@@ -1124,7 +1129,13 @@
         <v>9</v>
       </c>
       <c r="Y6" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA6">
+        <v>27433</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -1132,10 +1143,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -1144,25 +1155,25 @@
         <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="J7">
         <v>32039201</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s">
         <v>29</v>
-      </c>
-      <c r="L7" t="s">
-        <v>30</v>
       </c>
       <c r="M7" t="s">
         <v>20</v>
@@ -1171,25 +1182,25 @@
         <v>19</v>
       </c>
       <c r="O7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" t="s">
         <v>31</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>32</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>33</v>
       </c>
       <c r="R7">
         <v>967</v>
       </c>
       <c r="S7" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U7" t="s">
         <v>41</v>
-      </c>
-      <c r="T7" t="s">
-        <v>9</v>
-      </c>
-      <c r="U7" t="s">
-        <v>42</v>
       </c>
       <c r="W7" t="s">
         <v>8</v>
@@ -1206,10 +1217,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -1218,25 +1229,25 @@
         <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8">
         <v>32039201</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" t="s">
         <v>29</v>
-      </c>
-      <c r="L8" t="s">
-        <v>30</v>
       </c>
       <c r="M8" t="s">
         <v>20</v>
@@ -1245,13 +1256,13 @@
         <v>19</v>
       </c>
       <c r="O8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" t="s">
         <v>31</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>32</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>33</v>
       </c>
       <c r="R8">
         <v>967</v>
@@ -1260,13 +1271,13 @@
         <v>10</v>
       </c>
       <c r="T8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="W8" t="s">
         <v>8</v>
@@ -1283,10 +1294,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -1295,25 +1306,25 @@
         <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9">
         <v>32039201</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
         <v>29</v>
-      </c>
-      <c r="L9" t="s">
-        <v>30</v>
       </c>
       <c r="M9" t="s">
         <v>20</v>
@@ -1322,13 +1333,13 @@
         <v>19</v>
       </c>
       <c r="O9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" t="s">
         <v>31</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>32</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>33</v>
       </c>
       <c r="R9">
         <v>967</v>
@@ -1340,7 +1351,7 @@
         <v>9</v>
       </c>
       <c r="U9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W9" t="s">
         <v>8</v>
@@ -1357,10 +1368,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>63</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -1368,14 +1379,14 @@
       <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>26</v>
+      <c r="F10" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>23</v>
@@ -1383,11 +1394,11 @@
       <c r="J10">
         <v>32039201</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
         <v>29</v>
-      </c>
-      <c r="L10" t="s">
-        <v>30</v>
       </c>
       <c r="M10" t="s">
         <v>20</v>
@@ -1396,25 +1407,25 @@
         <v>19</v>
       </c>
       <c r="O10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" t="s">
         <v>31</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>32</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>33</v>
       </c>
       <c r="R10">
         <v>967</v>
       </c>
       <c r="S10" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="T10" t="s">
         <v>9</v>
       </c>
       <c r="U10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="W10" t="s">
         <v>8</v>
@@ -1431,10 +1442,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
@@ -1443,13 +1454,13 @@
         <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>23</v>
@@ -1457,11 +1468,11 @@
       <c r="J11">
         <v>32039201</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" t="s">
         <v>29</v>
-      </c>
-      <c r="L11" t="s">
-        <v>30</v>
       </c>
       <c r="M11" t="s">
         <v>20</v>
@@ -1470,13 +1481,13 @@
         <v>19</v>
       </c>
       <c r="O11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" t="s">
         <v>31</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>32</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>33</v>
       </c>
       <c r="R11">
         <v>967</v>
@@ -1488,7 +1499,7 @@
         <v>9</v>
       </c>
       <c r="U11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W11" t="s">
         <v>8</v>
@@ -1505,10 +1516,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
@@ -1516,14 +1527,14 @@
       <c r="E12" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>39</v>
+      <c r="F12" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>23</v>
@@ -1531,11 +1542,11 @@
       <c r="J12">
         <v>32039201</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" t="s">
         <v>29</v>
-      </c>
-      <c r="L12" t="s">
-        <v>30</v>
       </c>
       <c r="M12" t="s">
         <v>20</v>
@@ -1544,13 +1555,13 @@
         <v>19</v>
       </c>
       <c r="O12" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12" t="s">
         <v>31</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>32</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>33</v>
       </c>
       <c r="R12">
         <v>967</v>
@@ -1562,7 +1573,7 @@
         <v>9</v>
       </c>
       <c r="U12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W12" t="s">
         <v>8</v>
@@ -1579,10 +1590,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -1590,14 +1601,14 @@
       <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>43</v>
+      <c r="F13" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>23</v>
@@ -1605,11 +1616,11 @@
       <c r="J13">
         <v>32039201</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>29</v>
+      <c r="K13" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M13" t="s">
         <v>20</v>
@@ -1618,25 +1629,25 @@
         <v>19</v>
       </c>
       <c r="O13" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" t="s">
         <v>31</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>32</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>33</v>
       </c>
       <c r="R13">
         <v>967</v>
       </c>
       <c r="S13" t="s">
+        <v>40</v>
+      </c>
+      <c r="T13" t="s">
+        <v>9</v>
+      </c>
+      <c r="U13" t="s">
         <v>41</v>
-      </c>
-      <c r="T13" t="s">
-        <v>9</v>
-      </c>
-      <c r="U13" t="s">
-        <v>42</v>
       </c>
       <c r="W13" t="s">
         <v>8</v>
@@ -1653,10 +1664,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -1664,26 +1675,26 @@
       <c r="E14" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>57</v>
+      <c r="F14" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J14">
         <v>32039201</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>29</v>
+      <c r="K14" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M14" t="s">
         <v>20</v>
@@ -1692,28 +1703,28 @@
         <v>19</v>
       </c>
       <c r="O14" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" t="s">
         <v>31</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>32</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>33</v>
       </c>
       <c r="R14">
         <v>967</v>
       </c>
       <c r="S14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T14" t="s">
         <v>8</v>
       </c>
       <c r="U14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W14" t="s">
         <v>8</v>
@@ -1730,10 +1741,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
@@ -1741,14 +1752,14 @@
       <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>57</v>
+      <c r="F15" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>23</v>
@@ -1756,11 +1767,11 @@
       <c r="J15">
         <v>32039201</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>29</v>
+      <c r="K15" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M15" t="s">
         <v>20</v>
@@ -1769,28 +1780,28 @@
         <v>19</v>
       </c>
       <c r="O15" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15" t="s">
         <v>31</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>32</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>33</v>
       </c>
       <c r="R15">
         <v>967</v>
       </c>
       <c r="S15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T15" t="s">
         <v>8</v>
       </c>
       <c r="U15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W15" t="s">
         <v>8</v>
@@ -1807,10 +1818,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -1818,14 +1829,14 @@
       <c r="E16" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>57</v>
+      <c r="F16" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>23</v>
@@ -1833,11 +1844,11 @@
       <c r="J16">
         <v>32039201</v>
       </c>
-      <c r="K16" s="5" t="s">
-        <v>29</v>
+      <c r="K16" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M16" t="s">
         <v>20</v>
@@ -1846,28 +1857,28 @@
         <v>19</v>
       </c>
       <c r="O16" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" t="s">
         <v>31</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>32</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>33</v>
       </c>
       <c r="R16">
         <v>967</v>
       </c>
       <c r="S16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T16" t="s">
         <v>8</v>
       </c>
       <c r="U16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W16" t="s">
         <v>8</v>
@@ -1884,10 +1895,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
@@ -1895,14 +1906,14 @@
       <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>57</v>
+      <c r="F17" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>23</v>
@@ -1910,11 +1921,11 @@
       <c r="J17">
         <v>32039201</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>29</v>
+      <c r="K17" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="L17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M17" t="s">
         <v>20</v>
@@ -1923,28 +1934,28 @@
         <v>19</v>
       </c>
       <c r="O17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P17" t="s">
         <v>31</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>32</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>33</v>
       </c>
       <c r="R17">
         <v>967</v>
       </c>
       <c r="S17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T17" t="s">
         <v>8</v>
       </c>
       <c r="U17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W17" t="s">
         <v>8</v>
@@ -1970,8 +1981,9 @@
     <hyperlink ref="K4" r:id="rId10" xr:uid="{1D2D1264-1023-4FA6-BE44-61E74FDE4888}"/>
     <hyperlink ref="K5" r:id="rId11" xr:uid="{D9B9F4F4-8B02-461E-A9B6-DB381AC2D2CA}"/>
     <hyperlink ref="K3" r:id="rId12" xr:uid="{2B3E7683-CD5D-4D70-B265-DA9CC84D404C}"/>
+    <hyperlink ref="C10" r:id="rId13" xr:uid="{06AEB70B-6F80-4F82-9BED-4FCD994A9B6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
elimino smart folder No FT porque no es necesaria
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA548374-9ED5-4B2A-A1BA-1BD474CAAD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66408426-CF27-4779-B97F-B2C13FA95E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="79">
   <si>
     <t>Usuario</t>
   </si>
@@ -636,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,14 +1114,12 @@
         <v>40</v>
       </c>
       <c r="T6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U6" t="s">
-        <v>50</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="V6" s="1"/>
       <c r="W6" t="s">
         <v>8</v>
       </c>
@@ -1129,13 +1127,7 @@
         <v>9</v>
       </c>
       <c r="Y6" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA6">
-        <v>27433</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -1155,16 +1147,16 @@
         <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>59</v>
+      <c r="H7" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="J7">
         <v>32039201</v>
@@ -1173,7 +1165,7 @@
         <v>28</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="M7" t="s">
         <v>20</v>
@@ -1197,10 +1189,13 @@
         <v>40</v>
       </c>
       <c r="T7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U7" t="s">
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="W7" t="s">
         <v>8</v>
@@ -1209,7 +1204,13 @@
         <v>9</v>
       </c>
       <c r="Y7" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA7">
+        <v>27433</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -1217,10 +1218,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>64</v>
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -1229,13 +1230,13 @@
         <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>60</v>
@@ -1268,16 +1269,13 @@
         <v>967</v>
       </c>
       <c r="S8" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="T8" t="s">
         <v>9</v>
       </c>
       <c r="U8" t="s">
-        <v>47</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="W8" t="s">
         <v>8</v>
@@ -1306,7 +1304,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>25</v>
@@ -1351,7 +1349,10 @@
         <v>9</v>
       </c>
       <c r="U9" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="W9" t="s">
         <v>8</v>
@@ -1380,16 +1381,16 @@
         <v>22</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="J10">
         <v>32039201</v>
@@ -1419,13 +1420,13 @@
         <v>967</v>
       </c>
       <c r="S10" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="T10" t="s">
         <v>9</v>
       </c>
       <c r="U10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="W10" t="s">
         <v>8</v>
@@ -1442,10 +1443,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
@@ -1454,13 +1455,13 @@
         <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>23</v>
@@ -1493,13 +1494,13 @@
         <v>967</v>
       </c>
       <c r="S11" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="T11" t="s">
         <v>9</v>
       </c>
       <c r="U11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="W11" t="s">
         <v>8</v>
@@ -1516,10 +1517,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
@@ -1527,14 +1528,14 @@
       <c r="E12" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>38</v>
+      <c r="F12" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>23</v>
@@ -1602,7 +1603,7 @@
         <v>22</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>25</v>
@@ -1620,7 +1621,7 @@
         <v>28</v>
       </c>
       <c r="L13" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="M13" t="s">
         <v>20</v>
@@ -1641,13 +1642,13 @@
         <v>967</v>
       </c>
       <c r="S13" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="T13" t="s">
         <v>9</v>
       </c>
       <c r="U13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="W13" t="s">
         <v>8</v>
@@ -1675,17 +1676,17 @@
       <c r="E14" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>56</v>
+      <c r="F14" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="J14">
         <v>32039201</v>
@@ -1718,13 +1719,10 @@
         <v>40</v>
       </c>
       <c r="T14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U14" t="s">
-        <v>47</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="W14" t="s">
         <v>8</v>
@@ -1762,7 +1760,7 @@
         <v>54</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="J15">
         <v>32039201</v>
@@ -1798,7 +1796,7 @@
         <v>8</v>
       </c>
       <c r="U15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>46</v>
@@ -1875,7 +1873,7 @@
         <v>8</v>
       </c>
       <c r="U16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="V16" s="1" t="s">
         <v>46</v>
@@ -1952,7 +1950,7 @@
         <v>8</v>
       </c>
       <c r="U17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V17" s="1" t="s">
         <v>46</v>
@@ -1964,26 +1962,104 @@
         <v>9</v>
       </c>
       <c r="Y17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18">
+        <v>32039201</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" t="s">
+        <v>43</v>
+      </c>
+      <c r="M18" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" t="s">
+        <v>30</v>
+      </c>
+      <c r="P18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>32</v>
+      </c>
+      <c r="R18">
+        <v>967</v>
+      </c>
+      <c r="S18" t="s">
+        <v>40</v>
+      </c>
+      <c r="T18" t="s">
+        <v>8</v>
+      </c>
+      <c r="U18" t="s">
+        <v>51</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W18" t="s">
+        <v>8</v>
+      </c>
+      <c r="X18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y18" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2:K11" r:id="rId1" display="aseguradosgw@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="K15" r:id="rId4" xr:uid="{E5730AC6-DEB3-403E-8BE4-644FB8267106}"/>
-    <hyperlink ref="K16" r:id="rId5" xr:uid="{67C405C4-28CD-422E-BD81-37AA4C28D1CA}"/>
-    <hyperlink ref="K17" r:id="rId6" xr:uid="{FA8DAD41-3741-44DF-8312-8E211C556F8E}"/>
-    <hyperlink ref="K14" r:id="rId7" xr:uid="{92154F16-4C17-4536-8E7D-117722F9116C}"/>
-    <hyperlink ref="C8" r:id="rId8" xr:uid="{8A1338AD-AF81-4402-80D1-7B2091B345A9}"/>
-    <hyperlink ref="C9" r:id="rId9" xr:uid="{9D2C11E9-C232-4D40-B990-68F7F6926D40}"/>
+    <hyperlink ref="K2:K12" r:id="rId1" display="aseguradosgw@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="K16" r:id="rId4" xr:uid="{E5730AC6-DEB3-403E-8BE4-644FB8267106}"/>
+    <hyperlink ref="K17" r:id="rId5" xr:uid="{67C405C4-28CD-422E-BD81-37AA4C28D1CA}"/>
+    <hyperlink ref="K18" r:id="rId6" xr:uid="{FA8DAD41-3741-44DF-8312-8E211C556F8E}"/>
+    <hyperlink ref="K15" r:id="rId7" xr:uid="{92154F16-4C17-4536-8E7D-117722F9116C}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{8A1338AD-AF81-4402-80D1-7B2091B345A9}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{9D2C11E9-C232-4D40-B990-68F7F6926D40}"/>
     <hyperlink ref="K4" r:id="rId10" xr:uid="{1D2D1264-1023-4FA6-BE44-61E74FDE4888}"/>
     <hyperlink ref="K5" r:id="rId11" xr:uid="{D9B9F4F4-8B02-461E-A9B6-DB381AC2D2CA}"/>
     <hyperlink ref="K3" r:id="rId12" xr:uid="{2B3E7683-CD5D-4D70-B265-DA9CC84D404C}"/>
-    <hyperlink ref="C10" r:id="rId13" xr:uid="{06AEB70B-6F80-4F82-9BED-4FCD994A9B6B}"/>
+    <hyperlink ref="C11" r:id="rId13" xr:uid="{06AEB70B-6F80-4F82-9BED-4FCD994A9B6B}"/>
+    <hyperlink ref="K6" r:id="rId14" xr:uid="{790AEDE7-AC71-452B-8D4F-9022FEE27F7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizo data para emisión de FT
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13CD74E-5823-4865-85B4-D4E1898798AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0498BF37-86E0-48F1-AB41-5E9AF3E37AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="83">
   <si>
     <t>Usuario</t>
   </si>
@@ -141,21 +141,12 @@
     <t>https://i-preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
   </si>
   <si>
-    <t>04440026375</t>
-  </si>
-  <si>
-    <t>31/03/2021</t>
-  </si>
-  <si>
     <t>Pérdidas parciales</t>
   </si>
   <si>
     <t>Parcial (Resto del Vehiculo)</t>
   </si>
   <si>
-    <t>04440026526</t>
-  </si>
-  <si>
     <t>Daño Parcial</t>
   </si>
   <si>
@@ -277,6 +268,12 @@
   </si>
   <si>
     <t xml:space="preserve">04104018841 </t>
+  </si>
+  <si>
+    <t>04104019009</t>
+  </si>
+  <si>
+    <t>20/09/2021</t>
   </si>
 </sst>
 </file>
@@ -306,7 +303,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +313,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,17 +362,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -654,7 +665,7 @@
   <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="F2:I3"/>
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +687,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
@@ -727,19 +738,19 @@
         <v>19</v>
       </c>
       <c r="R1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="S1" t="s">
         <v>5</v>
       </c>
       <c r="T1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="U1" t="s">
         <v>15</v>
       </c>
       <c r="V1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="W1" t="s">
         <v>6</v>
@@ -748,13 +759,13 @@
         <v>7</v>
       </c>
       <c r="Y1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Z1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AA1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -762,10 +773,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -774,16 +785,16 @@
         <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>82</v>
+      <c r="H2" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J2">
         <v>32039201</v>
@@ -792,7 +803,7 @@
         <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M2" t="s">
         <v>20</v>
@@ -813,13 +824,13 @@
         <v>967</v>
       </c>
       <c r="S2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T2" t="s">
         <v>9</v>
       </c>
       <c r="U2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" t="s">
@@ -837,10 +848,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -849,16 +860,16 @@
         <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>82</v>
+      <c r="H3" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J3">
         <v>32039201</v>
@@ -867,7 +878,7 @@
         <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M3" t="s">
         <v>20</v>
@@ -888,16 +899,16 @@
         <v>967</v>
       </c>
       <c r="S3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T3" t="s">
         <v>8</v>
       </c>
       <c r="U3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="W3" t="s">
         <v>8</v>
@@ -914,10 +925,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -926,16 +937,16 @@
         <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>78</v>
+      <c r="H4" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J4">
         <v>32039201</v>
@@ -944,7 +955,7 @@
         <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M4" t="s">
         <v>20</v>
@@ -965,13 +976,13 @@
         <v>967</v>
       </c>
       <c r="S4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T4" t="s">
         <v>9</v>
       </c>
       <c r="U4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" t="s">
@@ -984,7 +995,7 @@
         <v>8</v>
       </c>
       <c r="Z4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AA4">
         <v>27433</v>
@@ -995,10 +1006,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -1007,16 +1018,16 @@
         <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>73</v>
+      <c r="H5" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J5">
         <v>32039201</v>
@@ -1025,7 +1036,7 @@
         <v>28</v>
       </c>
       <c r="L5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M5" t="s">
         <v>20</v>
@@ -1046,13 +1057,13 @@
         <v>967</v>
       </c>
       <c r="S5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T5" t="s">
         <v>9</v>
       </c>
       <c r="U5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" t="s">
@@ -1065,7 +1076,7 @@
         <v>8</v>
       </c>
       <c r="Z5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -1073,10 +1084,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -1085,16 +1096,16 @@
         <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>64</v>
+      <c r="H6" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J6">
         <v>32039201</v>
@@ -1103,7 +1114,7 @@
         <v>28</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M6" t="s">
         <v>20</v>
@@ -1124,13 +1135,13 @@
         <v>967</v>
       </c>
       <c r="S6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T6" t="s">
         <v>9</v>
       </c>
       <c r="U6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" t="s">
@@ -1148,10 +1159,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -1160,16 +1171,16 @@
         <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>64</v>
+      <c r="H7" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J7">
         <v>32039201</v>
@@ -1178,7 +1189,7 @@
         <v>28</v>
       </c>
       <c r="L7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M7" t="s">
         <v>20</v>
@@ -1199,16 +1210,16 @@
         <v>967</v>
       </c>
       <c r="S7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T7" t="s">
         <v>8</v>
       </c>
       <c r="U7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="W7" t="s">
         <v>8</v>
@@ -1220,7 +1231,7 @@
         <v>8</v>
       </c>
       <c r="Z7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AA7">
         <v>27433</v>
@@ -1231,10 +1242,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -1243,16 +1254,16 @@
         <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J8">
         <v>32039201</v>
@@ -1282,13 +1293,13 @@
         <v>967</v>
       </c>
       <c r="S8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T8" t="s">
         <v>9</v>
       </c>
       <c r="U8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="W8" t="s">
         <v>8</v>
@@ -1305,10 +1316,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -1317,16 +1328,16 @@
         <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J9">
         <v>32039201</v>
@@ -1356,13 +1367,13 @@
         <v>967</v>
       </c>
       <c r="S9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T9" t="s">
         <v>9</v>
       </c>
       <c r="U9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="V9" s="1"/>
       <c r="W9" t="s">
@@ -1377,10 +1388,10 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
@@ -1389,16 +1400,16 @@
         <v>22</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J10">
         <v>32039201</v>
@@ -1428,13 +1439,13 @@
         <v>967</v>
       </c>
       <c r="S10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T10" t="s">
         <v>9</v>
       </c>
       <c r="U10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="V10" s="1"/>
       <c r="W10" t="s">
@@ -1447,7 +1458,7 @@
         <v>8</v>
       </c>
       <c r="Z10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AA10">
         <v>27433</v>
@@ -1458,10 +1469,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
@@ -1470,16 +1481,16 @@
         <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J11">
         <v>32039201</v>
@@ -1532,10 +1543,10 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
@@ -1544,13 +1555,13 @@
         <v>22</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>23</v>
@@ -1583,13 +1594,13 @@
         <v>967</v>
       </c>
       <c r="S12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T12" t="s">
         <v>9</v>
       </c>
       <c r="U12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="W12" t="s">
         <v>8</v>
@@ -1675,228 +1686,234 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="9">
+        <v>32039201</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" s="9">
+        <v>967</v>
+      </c>
+      <c r="S14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="T14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="V14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="X14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y14" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="2" t="s">
+      <c r="H15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J14">
+      <c r="J15" s="9">
         <v>32039201</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K15" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" t="s">
+      <c r="L15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="Q15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="R14">
+      <c r="R15" s="9">
         <v>967</v>
       </c>
-      <c r="S14" t="s">
-        <v>10</v>
-      </c>
-      <c r="T14" t="s">
-        <v>9</v>
-      </c>
-      <c r="U14" t="s">
-        <v>33</v>
-      </c>
-      <c r="W14" t="s">
-        <v>8</v>
-      </c>
-      <c r="X14" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y14" t="s">
+      <c r="S15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="T15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="V15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="X15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y15" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="16" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="F16" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15">
+      <c r="H16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="9">
         <v>32039201</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="R16" s="9">
+        <v>967</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="T16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="U16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="V16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="M15" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" t="s">
-        <v>30</v>
-      </c>
-      <c r="P15" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>32</v>
-      </c>
-      <c r="R15">
-        <v>967</v>
-      </c>
-      <c r="S15" t="s">
-        <v>40</v>
-      </c>
-      <c r="T15" t="s">
-        <v>9</v>
-      </c>
-      <c r="U15" t="s">
-        <v>41</v>
-      </c>
-      <c r="W15" t="s">
-        <v>8</v>
-      </c>
-      <c r="X15" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J16">
-        <v>32039201</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" t="s">
-        <v>43</v>
-      </c>
-      <c r="M16" t="s">
-        <v>20</v>
-      </c>
-      <c r="N16" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" t="s">
-        <v>30</v>
-      </c>
-      <c r="P16" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>32</v>
-      </c>
-      <c r="R16">
-        <v>967</v>
-      </c>
-      <c r="S16" t="s">
-        <v>40</v>
-      </c>
-      <c r="T16" t="s">
-        <v>8</v>
-      </c>
-      <c r="U16" t="s">
-        <v>47</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="W16" t="s">
-        <v>8</v>
-      </c>
-      <c r="X16" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y16" t="s">
+      <c r="W16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="X16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y16" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1905,10 +1922,10 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
@@ -1916,14 +1933,14 @@
       <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>56</v>
+      <c r="F17" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>23</v>
@@ -1935,7 +1952,7 @@
         <v>28</v>
       </c>
       <c r="L17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M17" t="s">
         <v>20</v>
@@ -1956,16 +1973,16 @@
         <v>967</v>
       </c>
       <c r="S17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T17" t="s">
         <v>8</v>
       </c>
       <c r="U17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="W17" t="s">
         <v>8</v>
@@ -1982,10 +1999,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
@@ -1993,14 +2010,14 @@
       <c r="E18" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>56</v>
+      <c r="F18" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>23</v>
@@ -2012,7 +2029,7 @@
         <v>28</v>
       </c>
       <c r="L18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M18" t="s">
         <v>20</v>
@@ -2033,16 +2050,16 @@
         <v>967</v>
       </c>
       <c r="S18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T18" t="s">
         <v>8</v>
       </c>
       <c r="U18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="W18" t="s">
         <v>8</v>
@@ -2059,10 +2076,10 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
@@ -2070,14 +2087,14 @@
       <c r="E19" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>56</v>
+      <c r="F19" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>23</v>
@@ -2089,7 +2106,7 @@
         <v>28</v>
       </c>
       <c r="L19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M19" t="s">
         <v>20</v>
@@ -2110,16 +2127,16 @@
         <v>967</v>
       </c>
       <c r="S19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T19" t="s">
         <v>8</v>
       </c>
       <c r="U19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="W19" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
agrego CLEAS para motor tercero
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDED50C-3EDB-4251-B78D-95AFB09CCDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAE667B-E94D-4175-8957-1FCD29B0B9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="84">
   <si>
     <t>Usuario</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>20/09/2021</t>
+  </si>
+  <si>
+    <t>Daños Totales por Accidente Economica</t>
   </si>
 </sst>
 </file>
@@ -664,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M16" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,7 +1751,7 @@
         <v>9</v>
       </c>
       <c r="U14" s="9" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="V14" s="10" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
generacion motor: correccion en danios para que acepte la opcion no y agregado de robo total
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAE667B-E94D-4175-8957-1FCD29B0B9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492BF43B-C5D6-4D4A-8036-948790EACFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="87">
   <si>
     <t>Usuario</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Correo</t>
   </si>
   <si>
-    <t>DetalleSiniestro</t>
-  </si>
-  <si>
     <t>CausaSiniestro</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>aseguradosgw@gmail.com</t>
   </si>
   <si>
-    <t>Daño Total</t>
-  </si>
-  <si>
     <t>CAPITAL</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>Parcial (Resto del Vehiculo)</t>
   </si>
   <si>
-    <t>Daño Parcial</t>
-  </si>
-  <si>
     <t>EsFastTrack</t>
   </si>
   <si>
@@ -276,7 +267,25 @@
     <t>20/09/2021</t>
   </si>
   <si>
-    <t>Daños Totales por Accidente Economica</t>
+    <t>TipoRobo</t>
+  </si>
+  <si>
+    <t>SubtipoRobo</t>
+  </si>
+  <si>
+    <t>Robo y/o Hurto en estacionamiento privado: de alquiler o Shopping/Supermercado/Evento/Taller</t>
+  </si>
+  <si>
+    <t>Robo y/o Hurto Total Estacionado en vía pública</t>
+  </si>
+  <si>
+    <t>Robo y/o Hurto Total Mano Armada</t>
+  </si>
+  <si>
+    <t>Robo Parcial</t>
+  </si>
+  <si>
+    <t>Robo Total</t>
   </si>
 </sst>
 </file>
@@ -665,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,23 +689,22 @@
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -708,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -726,7 +734,7 @@
         <v>13</v>
       </c>
       <c r="M1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N1" t="s">
         <v>16</v>
@@ -738,1416 +746,1371 @@
         <v>18</v>
       </c>
       <c r="Q1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="R1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="S1" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="T1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="U1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="V1" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="W1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X1" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="Y1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="Z1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="AA1" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J2">
         <v>32039201</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>19</v>
-      </c>
       <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" t="s">
         <v>30</v>
       </c>
-      <c r="P2" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2">
+      <c r="Q2">
         <v>967</v>
       </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
       <c r="S2" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="T2" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V2" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="U2" s="1"/>
+      <c r="V2" t="s">
+        <v>8</v>
+      </c>
       <c r="W2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X2" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J3">
         <v>32039201</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3">
+        <v>967</v>
+      </c>
+      <c r="R3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3">
-        <v>967</v>
-      </c>
-      <c r="S3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" t="s">
-        <v>8</v>
-      </c>
-      <c r="U3" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>43</v>
+      <c r="V3" t="s">
+        <v>8</v>
       </c>
       <c r="W3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X3" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J4">
         <v>32039201</v>
       </c>
       <c r="K4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" t="s">
         <v>28</v>
       </c>
-      <c r="L4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" t="s">
-        <v>19</v>
-      </c>
       <c r="O4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" t="s">
         <v>30</v>
       </c>
-      <c r="P4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>32</v>
-      </c>
-      <c r="R4">
+      <c r="Q4">
         <v>967</v>
       </c>
+      <c r="R4" t="s">
+        <v>36</v>
+      </c>
       <c r="S4" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="T4" t="s">
-        <v>9</v>
-      </c>
-      <c r="U4" t="s">
-        <v>39</v>
-      </c>
-      <c r="V4" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" t="s">
+        <v>8</v>
+      </c>
       <c r="W4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA4">
+        <v>85</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB4">
         <v>27433</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J5">
         <v>32039201</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
         <v>28</v>
       </c>
-      <c r="L5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" t="s">
-        <v>19</v>
-      </c>
       <c r="O5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" t="s">
         <v>30</v>
       </c>
-      <c r="P5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5">
+      <c r="Q5">
         <v>967</v>
       </c>
+      <c r="R5" t="s">
+        <v>36</v>
+      </c>
       <c r="S5" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="T5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U5" t="s">
-        <v>63</v>
-      </c>
-      <c r="V5" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" t="s">
+        <v>8</v>
+      </c>
       <c r="W5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y5" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>69</v>
+        <v>85</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J6">
         <v>32039201</v>
       </c>
       <c r="K6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" t="s">
         <v>28</v>
       </c>
-      <c r="L6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>19</v>
-      </c>
       <c r="O6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" t="s">
         <v>30</v>
       </c>
-      <c r="P6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>32</v>
-      </c>
-      <c r="R6">
+      <c r="Q6">
         <v>967</v>
       </c>
+      <c r="R6" t="s">
+        <v>36</v>
+      </c>
       <c r="S6" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="T6" t="s">
-        <v>9</v>
-      </c>
-      <c r="U6" t="s">
-        <v>39</v>
-      </c>
-      <c r="V6" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="U6" s="1"/>
+      <c r="V6" t="s">
+        <v>8</v>
+      </c>
       <c r="W6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X6" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J7">
         <v>32039201</v>
       </c>
       <c r="K7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" t="s">
         <v>28</v>
       </c>
-      <c r="L7" t="s">
+      <c r="O7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7">
+        <v>967</v>
+      </c>
+      <c r="R7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" t="s">
+        <v>44</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R7">
-        <v>967</v>
-      </c>
-      <c r="S7" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" t="s">
-        <v>8</v>
-      </c>
-      <c r="U7" t="s">
-        <v>47</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>43</v>
+      <c r="V7" t="s">
+        <v>8</v>
       </c>
       <c r="W7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA7">
+        <v>85</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB7">
         <v>27433</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J8">
         <v>32039201</v>
       </c>
       <c r="K8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" t="s">
         <v>28</v>
       </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
         <v>29</v>
       </c>
-      <c r="M8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>30</v>
       </c>
-      <c r="P8" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>32</v>
-      </c>
-      <c r="R8">
+      <c r="Q8">
         <v>967</v>
       </c>
+      <c r="R8" t="s">
+        <v>36</v>
+      </c>
       <c r="S8" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="T8" t="s">
-        <v>9</v>
-      </c>
-      <c r="U8" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="V8" t="s">
+        <v>8</v>
       </c>
       <c r="W8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X8" t="s">
         <v>9</v>
       </c>
-      <c r="Y8" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J9">
         <v>32039201</v>
       </c>
       <c r="K9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s">
         <v>28</v>
       </c>
-      <c r="L9" t="s">
+      <c r="O9" t="s">
         <v>29</v>
       </c>
-      <c r="M9" t="s">
+      <c r="P9" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9">
+        <v>967</v>
+      </c>
+      <c r="R9" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" s="1"/>
+      <c r="V9" t="s">
+        <v>8</v>
+      </c>
+      <c r="W9" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="N9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R9">
-        <v>967</v>
-      </c>
-      <c r="S9" t="s">
-        <v>38</v>
-      </c>
-      <c r="T9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U9" t="s">
-        <v>39</v>
-      </c>
-      <c r="V9" s="1"/>
-      <c r="W9" t="s">
-        <v>8</v>
-      </c>
-      <c r="X9" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J10">
         <v>32039201</v>
       </c>
       <c r="K10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" t="s">
         <v>28</v>
       </c>
-      <c r="L10" t="s">
+      <c r="O10" t="s">
         <v>29</v>
       </c>
-      <c r="M10" t="s">
+      <c r="P10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10">
+        <v>967</v>
+      </c>
+      <c r="R10" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" t="s">
+        <v>9</v>
+      </c>
+      <c r="T10" t="s">
+        <v>37</v>
+      </c>
+      <c r="U10" s="1"/>
+      <c r="V10" t="s">
+        <v>8</v>
+      </c>
+      <c r="W10" t="s">
+        <v>9</v>
+      </c>
+      <c r="X10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB10">
+        <v>27433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="N10" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>32</v>
-      </c>
-      <c r="R10">
-        <v>967</v>
-      </c>
-      <c r="S10" t="s">
-        <v>38</v>
-      </c>
-      <c r="T10" t="s">
-        <v>9</v>
-      </c>
-      <c r="U10" t="s">
-        <v>39</v>
-      </c>
-      <c r="V10" s="1"/>
-      <c r="W10" t="s">
-        <v>8</v>
-      </c>
-      <c r="X10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA10">
-        <v>27433</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J11">
         <v>32039201</v>
       </c>
       <c r="K11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" t="s">
         <v>28</v>
       </c>
-      <c r="L11" t="s">
+      <c r="O11" t="s">
         <v>29</v>
       </c>
-      <c r="M11" t="s">
+      <c r="P11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11">
+        <v>967</v>
+      </c>
+      <c r="R11" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" t="s">
+        <v>9</v>
+      </c>
+      <c r="T11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V11" t="s">
+        <v>8</v>
+      </c>
+      <c r="W11" t="s">
+        <v>9</v>
+      </c>
+      <c r="X11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="N11" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" t="s">
-        <v>30</v>
-      </c>
-      <c r="P11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>32</v>
-      </c>
-      <c r="R11">
-        <v>967</v>
-      </c>
-      <c r="S11" t="s">
-        <v>10</v>
-      </c>
-      <c r="T11" t="s">
-        <v>9</v>
-      </c>
-      <c r="U11" t="s">
-        <v>33</v>
-      </c>
-      <c r="W11" t="s">
-        <v>8</v>
-      </c>
-      <c r="X11" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="J12">
         <v>32039201</v>
       </c>
       <c r="K12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" t="s">
         <v>28</v>
       </c>
-      <c r="L12" t="s">
+      <c r="O12" t="s">
         <v>29</v>
       </c>
-      <c r="M12" t="s">
-        <v>20</v>
-      </c>
-      <c r="N12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>30</v>
       </c>
-      <c r="P12" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>32</v>
-      </c>
-      <c r="R12">
+      <c r="Q12">
         <v>967</v>
       </c>
+      <c r="R12" t="s">
+        <v>36</v>
+      </c>
       <c r="S12" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="T12" t="s">
-        <v>9</v>
-      </c>
-      <c r="U12" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="V12" t="s">
+        <v>8</v>
       </c>
       <c r="W12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X12" t="s">
         <v>9</v>
       </c>
-      <c r="Y12" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="J13">
         <v>32039201</v>
       </c>
       <c r="K13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" t="s">
         <v>28</v>
       </c>
-      <c r="L13" t="s">
+      <c r="O13" t="s">
         <v>29</v>
       </c>
-      <c r="M13" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>30</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13">
+        <v>967</v>
+      </c>
+      <c r="R13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" t="s">
+        <v>9</v>
+      </c>
+      <c r="T13" t="s">
         <v>31</v>
       </c>
-      <c r="Q13" t="s">
-        <v>32</v>
-      </c>
-      <c r="R13">
-        <v>967</v>
-      </c>
-      <c r="S13" t="s">
-        <v>10</v>
-      </c>
-      <c r="T13" t="s">
-        <v>9</v>
-      </c>
-      <c r="U13" t="s">
-        <v>33</v>
+      <c r="V13" t="s">
+        <v>8</v>
       </c>
       <c r="W13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X13" t="s">
         <v>9</v>
       </c>
-      <c r="Y13" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="14" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J14" s="9">
         <v>32039201</v>
       </c>
       <c r="K14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="O14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R14" s="9">
+      <c r="Q14" s="9">
         <v>967</v>
       </c>
       <c r="S14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U14" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="V14" s="10" t="s">
-        <v>43</v>
+        <v>9</v>
+      </c>
+      <c r="U14" s="10"/>
+      <c r="V14" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="W14" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X14" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y14" s="9" t="s">
-        <v>9</v>
+        <v>86</v>
+      </c>
+      <c r="Z14" s="9" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J15" s="9">
         <v>32039201</v>
       </c>
       <c r="K15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="O15" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R15" s="9">
+      <c r="Q15" s="9">
         <v>967</v>
       </c>
       <c r="S15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="T15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="U15" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="V15" s="10" t="s">
-        <v>43</v>
+        <v>9</v>
+      </c>
+      <c r="U15" s="10"/>
+      <c r="V15" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="W15" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X15" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y15" s="9" t="s">
-        <v>9</v>
+        <v>86</v>
+      </c>
+      <c r="Z15" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="F16" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J16" s="9">
         <v>32039201</v>
       </c>
       <c r="K16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="O16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P16" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R16" s="9">
+      <c r="Q16" s="9">
         <v>967</v>
       </c>
       <c r="S16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="V16" s="10" t="s">
-        <v>43</v>
+        <v>9</v>
+      </c>
+      <c r="U16" s="10"/>
+      <c r="V16" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="W16" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X16" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Y16" s="9" t="s">
-        <v>9</v>
+        <v>86</v>
+      </c>
+      <c r="Z16" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="G17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="J17">
         <v>32039201</v>
       </c>
       <c r="K17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" t="s">
         <v>28</v>
       </c>
-      <c r="L17" t="s">
+      <c r="O17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P17" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q17">
+        <v>967</v>
+      </c>
+      <c r="R17" t="s">
+        <v>36</v>
+      </c>
+      <c r="S17" t="s">
+        <v>8</v>
+      </c>
+      <c r="T17" t="s">
+        <v>43</v>
+      </c>
+      <c r="U17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M17" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" t="s">
-        <v>30</v>
-      </c>
-      <c r="P17" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>32</v>
-      </c>
-      <c r="R17">
-        <v>967</v>
-      </c>
-      <c r="S17" t="s">
-        <v>38</v>
-      </c>
-      <c r="T17" t="s">
-        <v>8</v>
-      </c>
-      <c r="U17" t="s">
-        <v>46</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>43</v>
+      <c r="V17" t="s">
+        <v>8</v>
       </c>
       <c r="W17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X17" t="s">
         <v>9</v>
       </c>
-      <c r="Y17" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="G18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="J18">
         <v>32039201</v>
       </c>
       <c r="K18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" t="s">
         <v>28</v>
       </c>
-      <c r="L18" t="s">
+      <c r="O18" t="s">
+        <v>29</v>
+      </c>
+      <c r="P18" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q18">
+        <v>967</v>
+      </c>
+      <c r="R18" t="s">
+        <v>36</v>
+      </c>
+      <c r="S18" t="s">
+        <v>8</v>
+      </c>
+      <c r="T18" t="s">
+        <v>44</v>
+      </c>
+      <c r="U18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M18" t="s">
-        <v>20</v>
-      </c>
-      <c r="N18" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18" t="s">
-        <v>30</v>
-      </c>
-      <c r="P18" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>32</v>
-      </c>
-      <c r="R18">
-        <v>967</v>
-      </c>
-      <c r="S18" t="s">
-        <v>38</v>
-      </c>
-      <c r="T18" t="s">
-        <v>8</v>
-      </c>
-      <c r="U18" t="s">
-        <v>47</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>43</v>
+      <c r="V18" t="s">
+        <v>8</v>
       </c>
       <c r="W18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X18" t="s">
         <v>9</v>
       </c>
-      <c r="Y18" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="G19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="J19">
         <v>32039201</v>
       </c>
       <c r="K19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" t="s">
+        <v>18</v>
+      </c>
+      <c r="N19" t="s">
         <v>28</v>
       </c>
-      <c r="L19" t="s">
+      <c r="O19" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q19">
+        <v>967</v>
+      </c>
+      <c r="R19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S19" t="s">
+        <v>8</v>
+      </c>
+      <c r="T19" t="s">
+        <v>45</v>
+      </c>
+      <c r="U19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M19" t="s">
-        <v>20</v>
-      </c>
-      <c r="N19" t="s">
-        <v>19</v>
-      </c>
-      <c r="O19" t="s">
-        <v>30</v>
-      </c>
-      <c r="P19" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>32</v>
-      </c>
-      <c r="R19">
-        <v>967</v>
-      </c>
-      <c r="S19" t="s">
-        <v>38</v>
-      </c>
-      <c r="T19" t="s">
-        <v>8</v>
-      </c>
-      <c r="U19" t="s">
-        <v>48</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>43</v>
+      <c r="V19" t="s">
+        <v>8</v>
       </c>
       <c r="W19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X19" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y19" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
arreglos en motor y motor tercero
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492BF43B-C5D6-4D4A-8036-948790EACFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014B55DD-CE66-4213-A3AC-AEB8CFADE132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="88">
   <si>
     <t>Usuario</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>Robo Total</t>
+  </si>
+  <si>
+    <t>Daños Totales por Accidente Economica</t>
   </si>
 </sst>
 </file>
@@ -674,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB19"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,6 +1389,9 @@
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
       <c r="B10" t="s">
         <v>56</v>
       </c>
@@ -1465,7 +1471,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>56</v>
@@ -1536,7 +1542,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
@@ -1605,9 +1611,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
@@ -1677,8 +1683,8 @@
       </c>
     </row>
     <row r="14" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>11</v>
+      <c r="A14">
+        <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>47</v>
@@ -1728,28 +1734,27 @@
       <c r="Q14" s="9">
         <v>967</v>
       </c>
+      <c r="R14" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="S14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="U14" s="10"/>
+      <c r="T14" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="V14" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W14" s="9" t="s">
         <v>9</v>
       </c>
       <c r="X14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y14" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z14" s="9" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15">
         <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -1800,28 +1805,27 @@
       <c r="Q15" s="9">
         <v>967</v>
       </c>
+      <c r="R15" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="S15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="U15" s="10"/>
+      <c r="T15" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="V15" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W15" s="9" t="s">
         <v>9</v>
       </c>
       <c r="X15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y15" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z15" s="9" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1836,17 +1840,17 @@
       <c r="E16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>78</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="11" t="s">
         <v>79</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="J16" s="9">
         <v>32039201</v>
@@ -1889,158 +1893,154 @@
         <v>86</v>
       </c>
       <c r="Z16" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="F17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="H17" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="9">
         <v>32039201</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="9">
         <v>967</v>
       </c>
-      <c r="R17" t="s">
-        <v>36</v>
-      </c>
-      <c r="S17" t="s">
-        <v>8</v>
-      </c>
-      <c r="T17" t="s">
-        <v>43</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V17" t="s">
-        <v>8</v>
-      </c>
-      <c r="W17" t="s">
-        <v>9</v>
-      </c>
-      <c r="X17" t="s">
-        <v>9</v>
+      <c r="S17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U17" s="10"/>
+      <c r="V17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="X17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y17" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z17" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="F18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18">
+      <c r="H18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="9">
         <v>32039201</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="P18" t="s">
+      <c r="P18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="9">
         <v>967</v>
       </c>
-      <c r="R18" t="s">
-        <v>36</v>
-      </c>
-      <c r="S18" t="s">
-        <v>8</v>
-      </c>
-      <c r="T18" t="s">
-        <v>44</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V18" t="s">
-        <v>8</v>
-      </c>
-      <c r="W18" t="s">
-        <v>9</v>
-      </c>
-      <c r="X18" t="s">
-        <v>9</v>
+      <c r="S18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U18" s="10"/>
+      <c r="V18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="X18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y18" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z18" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>8</v>
       </c>
       <c r="T19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="U19" s="1" t="s">
         <v>40</v>
@@ -2111,18 +2111,166 @@
         <v>9</v>
       </c>
       <c r="X19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20">
+        <v>32039201</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20" t="s">
+        <v>29</v>
+      </c>
+      <c r="P20" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q20">
+        <v>967</v>
+      </c>
+      <c r="R20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S20" t="s">
+        <v>8</v>
+      </c>
+      <c r="T20" t="s">
+        <v>44</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V20" t="s">
+        <v>8</v>
+      </c>
+      <c r="W20" t="s">
+        <v>9</v>
+      </c>
+      <c r="X20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21">
+        <v>32039201</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q21">
+        <v>967</v>
+      </c>
+      <c r="R21" t="s">
+        <v>36</v>
+      </c>
+      <c r="S21" t="s">
+        <v>8</v>
+      </c>
+      <c r="T21" t="s">
+        <v>45</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V21" t="s">
+        <v>8</v>
+      </c>
+      <c r="W21" t="s">
+        <v>9</v>
+      </c>
+      <c r="X21" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2:K13" r:id="rId1" display="aseguradosgw@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="K17" r:id="rId4" xr:uid="{E5730AC6-DEB3-403E-8BE4-644FB8267106}"/>
-    <hyperlink ref="K18" r:id="rId5" xr:uid="{67C405C4-28CD-422E-BD81-37AA4C28D1CA}"/>
-    <hyperlink ref="K19" r:id="rId6" xr:uid="{FA8DAD41-3741-44DF-8312-8E211C556F8E}"/>
-    <hyperlink ref="K16" r:id="rId7" xr:uid="{92154F16-4C17-4536-8E7D-117722F9116C}"/>
+    <hyperlink ref="K16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="K19" r:id="rId4" xr:uid="{E5730AC6-DEB3-403E-8BE4-644FB8267106}"/>
+    <hyperlink ref="K20" r:id="rId5" xr:uid="{67C405C4-28CD-422E-BD81-37AA4C28D1CA}"/>
+    <hyperlink ref="K21" r:id="rId6" xr:uid="{FA8DAD41-3741-44DF-8312-8E211C556F8E}"/>
+    <hyperlink ref="K18" r:id="rId7" xr:uid="{92154F16-4C17-4536-8E7D-117722F9116C}"/>
     <hyperlink ref="C9" r:id="rId8" xr:uid="{8A1338AD-AF81-4402-80D1-7B2091B345A9}"/>
     <hyperlink ref="C11" r:id="rId9" xr:uid="{9D2C11E9-C232-4D40-B990-68F7F6926D40}"/>
     <hyperlink ref="K4" r:id="rId10" xr:uid="{1D2D1264-1023-4FA6-BE44-61E74FDE4888}"/>
@@ -2132,8 +2280,10 @@
     <hyperlink ref="K6" r:id="rId14" xr:uid="{790AEDE7-AC71-452B-8D4F-9022FEE27F7A}"/>
     <hyperlink ref="C10" r:id="rId15" xr:uid="{32F0979C-5F88-4EBD-BC8C-AF3FCAC48DAC}"/>
     <hyperlink ref="K10" r:id="rId16" xr:uid="{52EF6F38-0006-40B0-8B38-30AD54A75818}"/>
+    <hyperlink ref="K14" r:id="rId17" xr:uid="{A3D73405-6991-449C-A6C2-4AB73FCB20CB}"/>
+    <hyperlink ref="K15" r:id="rId18" xr:uid="{8DFF4F72-1AAD-4113-AEA5-E2CDD7E15084}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data para generacion de siniestros
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014B55DD-CE66-4213-A3AC-AEB8CFADE132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDDF636-69F8-4D66-AB0F-81FC34CE4FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="87">
   <si>
     <t>Usuario</t>
   </si>
@@ -261,12 +261,6 @@
     <t xml:space="preserve">04104018841 </t>
   </si>
   <si>
-    <t>04104019009</t>
-  </si>
-  <si>
-    <t>20/09/2021</t>
-  </si>
-  <si>
     <t>TipoRobo</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
     <t>Robo y/o Hurto Total Estacionado en vía pública</t>
   </si>
   <si>
-    <t>Robo y/o Hurto Total Mano Armada</t>
-  </si>
-  <si>
     <t>Robo Parcial</t>
   </si>
   <si>
@@ -289,6 +280,12 @@
   </si>
   <si>
     <t>Daños Totales por Accidente Economica</t>
+  </si>
+  <si>
+    <t>24/09/2024</t>
+  </si>
+  <si>
+    <t>04104019214</t>
   </si>
 </sst>
 </file>
@@ -377,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -388,9 +385,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
@@ -677,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB21"/>
+  <dimension ref="A1:AB24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,10 +767,10 @@
         <v>61</v>
       </c>
       <c r="Y1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Z1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AA1" t="s">
         <v>63</v>
@@ -933,7 +927,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
@@ -1003,7 +997,7 @@
         <v>8</v>
       </c>
       <c r="Y4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AA4" t="s">
         <v>64</v>
@@ -1014,7 +1008,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
@@ -1084,7 +1078,7 @@
         <v>8</v>
       </c>
       <c r="Y5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AA5" t="s">
         <v>66</v>
@@ -1092,7 +1086,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>47</v>
@@ -1164,7 +1158,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>47</v>
@@ -1236,7 +1230,7 @@
         <v>8</v>
       </c>
       <c r="Y7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AA7" t="s">
         <v>64</v>
@@ -1247,7 +1241,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
@@ -1318,7 +1312,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>56</v>
@@ -1390,7 +1384,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>56</v>
@@ -1460,7 +1454,7 @@
         <v>8</v>
       </c>
       <c r="Y10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AA10" t="s">
         <v>64</v>
@@ -1471,7 +1465,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>56</v>
@@ -1542,7 +1536,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
@@ -1613,7 +1607,7 @@
     </row>
     <row r="13" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
@@ -1682,608 +1676,829 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="12" t="s">
+      <c r="H14" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>967</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="T14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="V14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X14" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>967</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="V15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>967</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="S16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="V16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X16" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>967</v>
+      </c>
+      <c r="R17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="S17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="U17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="V17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X17" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>967</v>
+      </c>
+      <c r="R18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="T18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="V18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X18" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>967</v>
+      </c>
+      <c r="R19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="T19" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="V19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X19" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>967</v>
+      </c>
+      <c r="S20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="U20" s="9"/>
+      <c r="V20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y20" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z20" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>967</v>
+      </c>
+      <c r="S21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="U21" s="9"/>
+      <c r="V21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y21" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z21" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J22">
         <v>32039201</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="L22" t="s">
         <v>19</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="M22" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N22" t="s">
         <v>28</v>
       </c>
-      <c r="O14" s="9" t="s">
+      <c r="O22" t="s">
         <v>29</v>
       </c>
-      <c r="P14" s="9" t="s">
+      <c r="P22" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="Q22">
         <v>967</v>
       </c>
-      <c r="R14" s="9" t="s">
+      <c r="R22" t="s">
         <v>36</v>
       </c>
-      <c r="S14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="T14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="V14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="W14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="X14" s="9" t="s">
+      <c r="S22" t="s">
+        <v>8</v>
+      </c>
+      <c r="T22" t="s">
+        <v>43</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V22" t="s">
+        <v>8</v>
+      </c>
+      <c r="W22" t="s">
+        <v>9</v>
+      </c>
+      <c r="X22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" s="9" t="s">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C23" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D23" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E23" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="10" t="s">
+      <c r="F23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="12" t="s">
+      <c r="H23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J23">
         <v>32039201</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="K23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L23" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="M23" t="s">
         <v>18</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N23" t="s">
         <v>28</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="O23" t="s">
         <v>29</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="P23" t="s">
         <v>30</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="Q23">
         <v>967</v>
       </c>
-      <c r="R15" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="S15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="T15" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="V15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="W15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="X15" s="9" t="s">
+      <c r="R23" t="s">
+        <v>36</v>
+      </c>
+      <c r="S23" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" t="s">
+        <v>44</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V23" t="s">
+        <v>8</v>
+      </c>
+      <c r="W23" t="s">
+        <v>9</v>
+      </c>
+      <c r="X23" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" s="9" t="s">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C24" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E24" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" s="10" t="s">
+      <c r="F24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I16" s="12" t="s">
+      <c r="H24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J24">
         <v>32039201</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="9" t="s">
+      <c r="L24" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="M24" t="s">
         <v>18</v>
       </c>
-      <c r="N16" s="9" t="s">
+      <c r="N24" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="O24" t="s">
         <v>29</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="P24" t="s">
         <v>30</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="Q24">
         <v>967</v>
       </c>
-      <c r="S16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U16" s="10"/>
-      <c r="V16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="W16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="X16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y16" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z16" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="9">
-        <v>32039201</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P17" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q17" s="9">
-        <v>967</v>
-      </c>
-      <c r="S17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U17" s="10"/>
-      <c r="V17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="W17" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="X17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y17" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z17" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="9">
-        <v>32039201</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q18" s="9">
-        <v>967</v>
-      </c>
-      <c r="S18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U18" s="10"/>
-      <c r="V18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="W18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="X18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y18" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z18" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19">
-        <v>32039201</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" t="s">
-        <v>18</v>
-      </c>
-      <c r="N19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O19" t="s">
-        <v>29</v>
-      </c>
-      <c r="P19" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q19">
-        <v>967</v>
-      </c>
-      <c r="R19" t="s">
+      <c r="R24" t="s">
         <v>36</v>
       </c>
-      <c r="S19" t="s">
-        <v>8</v>
-      </c>
-      <c r="T19" t="s">
-        <v>43</v>
-      </c>
-      <c r="U19" s="1" t="s">
+      <c r="S24" t="s">
+        <v>8</v>
+      </c>
+      <c r="T24" t="s">
+        <v>45</v>
+      </c>
+      <c r="U24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V19" t="s">
-        <v>8</v>
-      </c>
-      <c r="W19" t="s">
-        <v>9</v>
-      </c>
-      <c r="X19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J20">
-        <v>32039201</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L20" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" t="s">
-        <v>18</v>
-      </c>
-      <c r="N20" t="s">
-        <v>28</v>
-      </c>
-      <c r="O20" t="s">
-        <v>29</v>
-      </c>
-      <c r="P20" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q20">
-        <v>967</v>
-      </c>
-      <c r="R20" t="s">
-        <v>36</v>
-      </c>
-      <c r="S20" t="s">
-        <v>8</v>
-      </c>
-      <c r="T20" t="s">
-        <v>44</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V20" t="s">
-        <v>8</v>
-      </c>
-      <c r="W20" t="s">
-        <v>9</v>
-      </c>
-      <c r="X20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21">
-        <v>32039201</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" t="s">
-        <v>18</v>
-      </c>
-      <c r="N21" t="s">
-        <v>28</v>
-      </c>
-      <c r="O21" t="s">
-        <v>29</v>
-      </c>
-      <c r="P21" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q21">
-        <v>967</v>
-      </c>
-      <c r="R21" t="s">
-        <v>36</v>
-      </c>
-      <c r="S21" t="s">
-        <v>8</v>
-      </c>
-      <c r="T21" t="s">
-        <v>45</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="V21" t="s">
-        <v>8</v>
-      </c>
-      <c r="W21" t="s">
-        <v>9</v>
-      </c>
-      <c r="X21" t="s">
+      <c r="V24" t="s">
+        <v>8</v>
+      </c>
+      <c r="W24" t="s">
+        <v>9</v>
+      </c>
+      <c r="X24" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2:K13" r:id="rId1" display="aseguradosgw@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="K19" r:id="rId4" xr:uid="{E5730AC6-DEB3-403E-8BE4-644FB8267106}"/>
-    <hyperlink ref="K20" r:id="rId5" xr:uid="{67C405C4-28CD-422E-BD81-37AA4C28D1CA}"/>
-    <hyperlink ref="K21" r:id="rId6" xr:uid="{FA8DAD41-3741-44DF-8312-8E211C556F8E}"/>
-    <hyperlink ref="K18" r:id="rId7" xr:uid="{92154F16-4C17-4536-8E7D-117722F9116C}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{8A1338AD-AF81-4402-80D1-7B2091B345A9}"/>
-    <hyperlink ref="C11" r:id="rId9" xr:uid="{9D2C11E9-C232-4D40-B990-68F7F6926D40}"/>
-    <hyperlink ref="K4" r:id="rId10" xr:uid="{1D2D1264-1023-4FA6-BE44-61E74FDE4888}"/>
-    <hyperlink ref="K5" r:id="rId11" xr:uid="{D9B9F4F4-8B02-461E-A9B6-DB381AC2D2CA}"/>
-    <hyperlink ref="K3" r:id="rId12" xr:uid="{2B3E7683-CD5D-4D70-B265-DA9CC84D404C}"/>
-    <hyperlink ref="C12" r:id="rId13" xr:uid="{06AEB70B-6F80-4F82-9BED-4FCD994A9B6B}"/>
-    <hyperlink ref="K6" r:id="rId14" xr:uid="{790AEDE7-AC71-452B-8D4F-9022FEE27F7A}"/>
-    <hyperlink ref="C10" r:id="rId15" xr:uid="{32F0979C-5F88-4EBD-BC8C-AF3FCAC48DAC}"/>
-    <hyperlink ref="K10" r:id="rId16" xr:uid="{52EF6F38-0006-40B0-8B38-30AD54A75818}"/>
-    <hyperlink ref="K14" r:id="rId17" xr:uid="{A3D73405-6991-449C-A6C2-4AB73FCB20CB}"/>
-    <hyperlink ref="K15" r:id="rId18" xr:uid="{8DFF4F72-1AAD-4113-AEA5-E2CDD7E15084}"/>
+    <hyperlink ref="K20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K21" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="K22" r:id="rId4" xr:uid="{E5730AC6-DEB3-403E-8BE4-644FB8267106}"/>
+    <hyperlink ref="K23" r:id="rId5" xr:uid="{67C405C4-28CD-422E-BD81-37AA4C28D1CA}"/>
+    <hyperlink ref="K24" r:id="rId6" xr:uid="{FA8DAD41-3741-44DF-8312-8E211C556F8E}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{8A1338AD-AF81-4402-80D1-7B2091B345A9}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{9D2C11E9-C232-4D40-B990-68F7F6926D40}"/>
+    <hyperlink ref="K4" r:id="rId9" xr:uid="{1D2D1264-1023-4FA6-BE44-61E74FDE4888}"/>
+    <hyperlink ref="K5" r:id="rId10" xr:uid="{D9B9F4F4-8B02-461E-A9B6-DB381AC2D2CA}"/>
+    <hyperlink ref="K3" r:id="rId11" xr:uid="{2B3E7683-CD5D-4D70-B265-DA9CC84D404C}"/>
+    <hyperlink ref="C12" r:id="rId12" xr:uid="{06AEB70B-6F80-4F82-9BED-4FCD994A9B6B}"/>
+    <hyperlink ref="K6" r:id="rId13" xr:uid="{790AEDE7-AC71-452B-8D4F-9022FEE27F7A}"/>
+    <hyperlink ref="C10" r:id="rId14" xr:uid="{32F0979C-5F88-4EBD-BC8C-AF3FCAC48DAC}"/>
+    <hyperlink ref="K10" r:id="rId15" xr:uid="{52EF6F38-0006-40B0-8B38-30AD54A75818}"/>
+    <hyperlink ref="K14" r:id="rId16" xr:uid="{A3D73405-6991-449C-A6C2-4AB73FCB20CB}"/>
+    <hyperlink ref="K16" r:id="rId17" xr:uid="{8DFF4F72-1AAD-4113-AEA5-E2CDD7E15084}"/>
+    <hyperlink ref="K15" r:id="rId18" xr:uid="{311DD90C-ABFD-423E-810F-03E025079EB3}"/>
+    <hyperlink ref="K17" r:id="rId19" xr:uid="{EB5EBC38-48DF-47AA-89C5-E5147A2CCADD}"/>
+    <hyperlink ref="K18" r:id="rId20" xr:uid="{77802F46-9803-41E9-9477-705FD5AF7D30}"/>
+    <hyperlink ref="K19" r:id="rId21" xr:uid="{AD32246E-C00F-4FB6-93FB-7743ED98E74F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualización de data para generación preprod
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2E389D-8CD2-48CB-A900-67DA3C59536F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B138D5D4-78F6-4DEB-887B-43758FE5851A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="82">
   <si>
     <t>Usuario</t>
   </si>
@@ -192,9 +192,6 @@
     <t>12:30</t>
   </si>
   <si>
-    <t>04104016408</t>
-  </si>
-  <si>
     <t>preproducciongestion.segurossura.com.ar</t>
   </si>
   <si>
@@ -231,30 +228,12 @@
     <t>08/08/2021</t>
   </si>
   <si>
-    <t>04104016685</t>
-  </si>
-  <si>
-    <t>01/06/2021</t>
-  </si>
-  <si>
-    <t>30/04/2021</t>
-  </si>
-  <si>
     <t>04104018682</t>
   </si>
   <si>
     <t>25/02/2022</t>
   </si>
   <si>
-    <t>08:30</t>
-  </si>
-  <si>
-    <t>15/06/2021</t>
-  </si>
-  <si>
-    <t>04104016746</t>
-  </si>
-  <si>
     <t>22/06/2021</t>
   </si>
   <si>
@@ -286,6 +265,12 @@
   </si>
   <si>
     <t>04104019214</t>
+  </si>
+  <si>
+    <t>04104017129</t>
+  </si>
+  <si>
+    <t>08/07/2021</t>
   </si>
 </sst>
 </file>
@@ -315,7 +300,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,7 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -390,6 +381,11 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -673,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,19 +760,19 @@
         <v>7</v>
       </c>
       <c r="X1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB1" t="s">
         <v>61</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -796,13 +792,13 @@
         <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>42</v>
@@ -868,13 +864,13 @@
         <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>42</v>
@@ -942,13 +938,13 @@
         <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>42</v>
@@ -997,10 +993,10 @@
         <v>8</v>
       </c>
       <c r="Y4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="AA4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB4">
         <v>27433</v>
@@ -1023,13 +1019,13 @@
         <v>21</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>42</v>
@@ -1065,7 +1061,7 @@
         <v>9</v>
       </c>
       <c r="T5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U5" s="1"/>
       <c r="V5" t="s">
@@ -1078,10 +1074,10 @@
         <v>8</v>
       </c>
       <c r="Y5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="AA5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -1101,13 +1097,13 @@
         <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>42</v>
@@ -1173,13 +1169,13 @@
         <v>21</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>42</v>
@@ -1230,10 +1226,10 @@
         <v>8</v>
       </c>
       <c r="Y7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="AA7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB7">
         <v>27433</v>
@@ -1310,298 +1306,295 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="2" t="s">
+      <c r="H9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="13">
+        <v>32039201</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>967</v>
+      </c>
+      <c r="R9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" s="16"/>
+      <c r="V9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="X9" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="13">
+        <v>32039201</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="13">
+        <v>967</v>
+      </c>
+      <c r="R10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="T10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="U10" s="16"/>
+      <c r="V10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="X10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z10" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="J9">
+    </row>
+    <row r="11" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="13">
         <v>32039201</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="Q9">
+      <c r="Q11" s="13">
         <v>967</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="V11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X11" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="13">
+        <v>32039201</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>967</v>
+      </c>
+      <c r="R12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="S9" t="s">
-        <v>9</v>
-      </c>
-      <c r="T9" t="s">
+      <c r="S12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="U9" s="1"/>
-      <c r="V9" t="s">
-        <v>8</v>
-      </c>
-      <c r="W9" t="s">
-        <v>9</v>
-      </c>
-      <c r="X9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J10">
-        <v>32039201</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" t="s">
-        <v>29</v>
-      </c>
-      <c r="P10" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10">
-        <v>967</v>
-      </c>
-      <c r="R10" t="s">
-        <v>36</v>
-      </c>
-      <c r="S10" t="s">
-        <v>9</v>
-      </c>
-      <c r="T10" t="s">
-        <v>37</v>
-      </c>
-      <c r="U10" s="1"/>
-      <c r="V10" t="s">
-        <v>8</v>
-      </c>
-      <c r="W10" t="s">
-        <v>9</v>
-      </c>
-      <c r="X10" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB10">
-        <v>27433</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11">
-        <v>32039201</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q11">
-        <v>967</v>
-      </c>
-      <c r="R11" t="s">
-        <v>10</v>
-      </c>
-      <c r="S11" t="s">
-        <v>9</v>
-      </c>
-      <c r="T11" t="s">
-        <v>31</v>
-      </c>
-      <c r="V11" t="s">
-        <v>8</v>
-      </c>
-      <c r="W11" t="s">
-        <v>9</v>
-      </c>
-      <c r="X11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12">
-        <v>32039201</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q12">
-        <v>967</v>
-      </c>
-      <c r="R12" t="s">
-        <v>36</v>
-      </c>
-      <c r="S12" t="s">
-        <v>9</v>
-      </c>
-      <c r="T12" t="s">
-        <v>37</v>
-      </c>
-      <c r="V12" t="s">
-        <v>8</v>
-      </c>
-      <c r="W12" t="s">
-        <v>9</v>
-      </c>
-      <c r="X12" t="s">
+      <c r="V12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X12" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1693,13 +1686,13 @@
         <v>21</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>42</v>
@@ -1764,13 +1757,13 @@
         <v>21</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>42</v>
@@ -1835,13 +1828,13 @@
         <v>21</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>42</v>
@@ -1909,13 +1902,13 @@
         <v>21</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I17" s="11" t="s">
         <v>42</v>
@@ -1983,13 +1976,13 @@
         <v>21</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>42</v>
@@ -2025,7 +2018,7 @@
         <v>9</v>
       </c>
       <c r="T18" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="V18" s="8" t="s">
         <v>8</v>
@@ -2054,13 +2047,13 @@
         <v>21</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I19" s="11" t="s">
         <v>42</v>
@@ -2096,7 +2089,7 @@
         <v>9</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="V19" s="8" t="s">
         <v>8</v>
@@ -2125,13 +2118,13 @@
         <v>21</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>42</v>
@@ -2174,10 +2167,10 @@
         <v>8</v>
       </c>
       <c r="Y20" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Z20" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2197,13 +2190,13 @@
         <v>21</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>42</v>
@@ -2246,10 +2239,10 @@
         <v>8</v>
       </c>
       <c r="Y21" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Z21" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
modifico data motor y test run motorSinUBER para sacar motor tercero
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B138D5D4-78F6-4DEB-887B-43758FE5851A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6186E86-2567-4ABD-AC09-6930FA012DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="82">
   <si>
     <t>Usuario</t>
   </si>
@@ -267,10 +267,10 @@
     <t>04104019214</t>
   </si>
   <si>
-    <t>04104017129</t>
-  </si>
-  <si>
     <t>08/07/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04104017130 </t>
   </si>
 </sst>
 </file>
@@ -667,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB24"/>
+  <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,13 +1323,13 @@
         <v>21</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>42</v>
@@ -1359,13 +1359,13 @@
         <v>967</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="S9" s="13" t="s">
         <v>9</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="U9" s="16"/>
       <c r="V9" s="13" t="s">
@@ -1380,7 +1380,7 @@
     </row>
     <row r="10" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>55</v>
@@ -1395,13 +1395,13 @@
         <v>21</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>42</v>
@@ -1431,15 +1431,14 @@
         <v>967</v>
       </c>
       <c r="R10" s="13" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="S10" s="13" t="s">
         <v>9</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="U10" s="16"/>
+        <v>31</v>
+      </c>
       <c r="V10" s="13" t="s">
         <v>8</v>
       </c>
@@ -1447,18 +1446,12 @@
         <v>9</v>
       </c>
       <c r="X10" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y10" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z10" s="13" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>55</v>
@@ -1473,13 +1466,13 @@
         <v>21</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>42</v>
@@ -1509,27 +1502,34 @@
         <v>967</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>31</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="U11" s="16"/>
       <c r="V11" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="W11" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X11" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="Y11" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z11" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>55</v>
@@ -1544,13 +1544,13 @@
         <v>21</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>42</v>
@@ -1589,305 +1589,309 @@
         <v>37</v>
       </c>
       <c r="V12" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="W12" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X12" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="Y12" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z12" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="13">
+        <v>32039201</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="13">
+        <v>967</v>
+      </c>
+      <c r="R13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="T13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="U13" s="16"/>
+      <c r="V13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X13" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>10</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="13">
+        <v>32039201</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="13">
+        <v>967</v>
+      </c>
+      <c r="R14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="T14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="V14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="X14" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>11</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="13">
+        <v>32039201</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="13">
+        <v>967</v>
+      </c>
+      <c r="R15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="T15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="V15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="X15" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>20</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E16" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J13">
+      <c r="J16">
         <v>32039201</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L16" t="s">
         <v>19</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M16" t="s">
         <v>18</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N16" t="s">
         <v>28</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O16" t="s">
         <v>29</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P16" t="s">
         <v>30</v>
       </c>
-      <c r="Q13">
+      <c r="Q16">
         <v>967</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R16" t="s">
         <v>10</v>
       </c>
-      <c r="S13" t="s">
-        <v>9</v>
-      </c>
-      <c r="T13" t="s">
+      <c r="S16" t="s">
+        <v>9</v>
+      </c>
+      <c r="T16" t="s">
         <v>31</v>
       </c>
-      <c r="V13" t="s">
-        <v>8</v>
-      </c>
-      <c r="W13" t="s">
-        <v>9</v>
-      </c>
-      <c r="X13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J14" s="8">
-        <v>32039201</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>967</v>
-      </c>
-      <c r="R14" t="s">
-        <v>10</v>
-      </c>
-      <c r="S14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="T14" t="s">
-        <v>31</v>
-      </c>
-      <c r="V14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="W14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="X14" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J15" s="8">
-        <v>32039201</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q15" s="8">
-        <v>967</v>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="T15" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="V15" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="W15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="X15" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="8">
-        <v>32039201</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>967</v>
-      </c>
-      <c r="R16" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="S16" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="T16" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="V16" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="W16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="X16" s="8" t="s">
+      <c r="V16" t="s">
+        <v>8</v>
+      </c>
+      <c r="W16" t="s">
+        <v>9</v>
+      </c>
+      <c r="X16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>47</v>
@@ -1937,23 +1941,20 @@
       <c r="Q17" s="8">
         <v>967</v>
       </c>
-      <c r="R17" s="8" t="s">
-        <v>36</v>
+      <c r="R17" t="s">
+        <v>10</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="T17" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="U17" s="9" t="s">
-        <v>40</v>
+        <v>9</v>
+      </c>
+      <c r="T17" t="s">
+        <v>31</v>
       </c>
       <c r="V17" s="8" t="s">
         <v>8</v>
       </c>
       <c r="W17" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X17" s="8" t="s">
         <v>9</v>
@@ -1961,7 +1962,7 @@
     </row>
     <row r="18" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>47</v>
@@ -2012,13 +2013,13 @@
         <v>967</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S18" s="8" t="s">
         <v>9</v>
       </c>
       <c r="T18" s="8" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="V18" s="8" t="s">
         <v>8</v>
@@ -2032,7 +2033,7 @@
     </row>
     <row r="19" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>47</v>
@@ -2083,13 +2084,16 @@
         <v>967</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S19" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>77</v>
+        <v>43</v>
+      </c>
+      <c r="U19" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="V19" s="8" t="s">
         <v>8</v>
@@ -2103,7 +2107,7 @@
     </row>
     <row r="20" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>47</v>
@@ -2153,29 +2157,31 @@
       <c r="Q20" s="8">
         <v>967</v>
       </c>
+      <c r="R20" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="S20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="U20" s="9"/>
+        <v>8</v>
+      </c>
+      <c r="T20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="U20" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="V20" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W20" s="8" t="s">
         <v>9</v>
       </c>
       <c r="X20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y20" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z20" s="8" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>47</v>
@@ -2225,273 +2231,493 @@
       <c r="Q21" s="8">
         <v>967</v>
       </c>
+      <c r="R21" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="S21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="U21" s="9"/>
+      <c r="T21" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="V21" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W21" s="8" t="s">
         <v>9</v>
       </c>
       <c r="X21" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y21" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>967</v>
+      </c>
+      <c r="R22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="T22" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X22" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>967</v>
+      </c>
+      <c r="S23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="U23" s="9"/>
+      <c r="V23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y23" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Z21" s="8" t="s">
+      <c r="Z23" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="8">
+        <v>32039201</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>967</v>
+      </c>
+      <c r="S24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="U24" s="9"/>
+      <c r="V24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="W24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="X24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z24" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>46</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>20</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E25" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J22">
+      <c r="J25">
         <v>32039201</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L25" t="s">
         <v>19</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M25" t="s">
         <v>18</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N25" t="s">
         <v>28</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O25" t="s">
         <v>29</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P25" t="s">
         <v>30</v>
       </c>
-      <c r="Q22">
+      <c r="Q25">
         <v>967</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R25" t="s">
         <v>36</v>
       </c>
-      <c r="S22" t="s">
-        <v>8</v>
-      </c>
-      <c r="T22" t="s">
+      <c r="S25" t="s">
+        <v>8</v>
+      </c>
+      <c r="T25" t="s">
         <v>43</v>
       </c>
-      <c r="U22" s="1" t="s">
+      <c r="U25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V22" t="s">
-        <v>8</v>
-      </c>
-      <c r="W22" t="s">
-        <v>9</v>
-      </c>
-      <c r="X22" t="s">
+      <c r="V25" t="s">
+        <v>8</v>
+      </c>
+      <c r="W25" t="s">
+        <v>9</v>
+      </c>
+      <c r="X25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>20</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J23">
+      <c r="J26">
         <v>32039201</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L26" t="s">
         <v>19</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M26" t="s">
         <v>18</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N26" t="s">
         <v>28</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O26" t="s">
         <v>29</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P26" t="s">
         <v>30</v>
       </c>
-      <c r="Q23">
+      <c r="Q26">
         <v>967</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R26" t="s">
         <v>36</v>
       </c>
-      <c r="S23" t="s">
-        <v>8</v>
-      </c>
-      <c r="T23" t="s">
+      <c r="S26" t="s">
+        <v>8</v>
+      </c>
+      <c r="T26" t="s">
         <v>44</v>
       </c>
-      <c r="U23" s="1" t="s">
+      <c r="U26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V23" t="s">
-        <v>8</v>
-      </c>
-      <c r="W23" t="s">
-        <v>9</v>
-      </c>
-      <c r="X23" t="s">
+      <c r="V26" t="s">
+        <v>8</v>
+      </c>
+      <c r="W26" t="s">
+        <v>9</v>
+      </c>
+      <c r="X26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>47</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>46</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>20</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E27" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J24">
+      <c r="J27">
         <v>32039201</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L27" t="s">
         <v>19</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M27" t="s">
         <v>18</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N27" t="s">
         <v>28</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O27" t="s">
         <v>29</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P27" t="s">
         <v>30</v>
       </c>
-      <c r="Q24">
+      <c r="Q27">
         <v>967</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R27" t="s">
         <v>36</v>
       </c>
-      <c r="S24" t="s">
-        <v>8</v>
-      </c>
-      <c r="T24" t="s">
+      <c r="S27" t="s">
+        <v>8</v>
+      </c>
+      <c r="T27" t="s">
         <v>45</v>
       </c>
-      <c r="U24" s="1" t="s">
+      <c r="U27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V24" t="s">
-        <v>8</v>
-      </c>
-      <c r="W24" t="s">
-        <v>9</v>
-      </c>
-      <c r="X24" t="s">
+      <c r="V27" t="s">
+        <v>8</v>
+      </c>
+      <c r="W27" t="s">
+        <v>9</v>
+      </c>
+      <c r="X27" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2:K13" r:id="rId1" display="aseguradosgw@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K21" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="K22" r:id="rId4" xr:uid="{E5730AC6-DEB3-403E-8BE4-644FB8267106}"/>
-    <hyperlink ref="K23" r:id="rId5" xr:uid="{67C405C4-28CD-422E-BD81-37AA4C28D1CA}"/>
-    <hyperlink ref="K24" r:id="rId6" xr:uid="{FA8DAD41-3741-44DF-8312-8E211C556F8E}"/>
+    <hyperlink ref="K2:K16" r:id="rId1" display="aseguradosgw@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K23" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="K25" r:id="rId4" xr:uid="{E5730AC6-DEB3-403E-8BE4-644FB8267106}"/>
+    <hyperlink ref="K26" r:id="rId5" xr:uid="{67C405C4-28CD-422E-BD81-37AA4C28D1CA}"/>
+    <hyperlink ref="K27" r:id="rId6" xr:uid="{FA8DAD41-3741-44DF-8312-8E211C556F8E}"/>
     <hyperlink ref="C9" r:id="rId7" xr:uid="{8A1338AD-AF81-4402-80D1-7B2091B345A9}"/>
-    <hyperlink ref="C11" r:id="rId8" xr:uid="{9D2C11E9-C232-4D40-B990-68F7F6926D40}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{9D2C11E9-C232-4D40-B990-68F7F6926D40}"/>
     <hyperlink ref="K4" r:id="rId9" xr:uid="{1D2D1264-1023-4FA6-BE44-61E74FDE4888}"/>
     <hyperlink ref="K5" r:id="rId10" xr:uid="{D9B9F4F4-8B02-461E-A9B6-DB381AC2D2CA}"/>
     <hyperlink ref="K3" r:id="rId11" xr:uid="{2B3E7683-CD5D-4D70-B265-DA9CC84D404C}"/>
-    <hyperlink ref="C12" r:id="rId12" xr:uid="{06AEB70B-6F80-4F82-9BED-4FCD994A9B6B}"/>
+    <hyperlink ref="C15" r:id="rId12" xr:uid="{06AEB70B-6F80-4F82-9BED-4FCD994A9B6B}"/>
     <hyperlink ref="K6" r:id="rId13" xr:uid="{790AEDE7-AC71-452B-8D4F-9022FEE27F7A}"/>
-    <hyperlink ref="C10" r:id="rId14" xr:uid="{32F0979C-5F88-4EBD-BC8C-AF3FCAC48DAC}"/>
-    <hyperlink ref="K10" r:id="rId15" xr:uid="{52EF6F38-0006-40B0-8B38-30AD54A75818}"/>
-    <hyperlink ref="K14" r:id="rId16" xr:uid="{A3D73405-6991-449C-A6C2-4AB73FCB20CB}"/>
-    <hyperlink ref="K16" r:id="rId17" xr:uid="{8DFF4F72-1AAD-4113-AEA5-E2CDD7E15084}"/>
-    <hyperlink ref="K15" r:id="rId18" xr:uid="{311DD90C-ABFD-423E-810F-03E025079EB3}"/>
-    <hyperlink ref="K17" r:id="rId19" xr:uid="{EB5EBC38-48DF-47AA-89C5-E5147A2CCADD}"/>
-    <hyperlink ref="K18" r:id="rId20" xr:uid="{77802F46-9803-41E9-9477-705FD5AF7D30}"/>
-    <hyperlink ref="K19" r:id="rId21" xr:uid="{AD32246E-C00F-4FB6-93FB-7743ED98E74F}"/>
+    <hyperlink ref="C11" r:id="rId14" xr:uid="{32F0979C-5F88-4EBD-BC8C-AF3FCAC48DAC}"/>
+    <hyperlink ref="K11" r:id="rId15" xr:uid="{52EF6F38-0006-40B0-8B38-30AD54A75818}"/>
+    <hyperlink ref="K17" r:id="rId16" xr:uid="{A3D73405-6991-449C-A6C2-4AB73FCB20CB}"/>
+    <hyperlink ref="K19" r:id="rId17" xr:uid="{8DFF4F72-1AAD-4113-AEA5-E2CDD7E15084}"/>
+    <hyperlink ref="K18" r:id="rId18" xr:uid="{311DD90C-ABFD-423E-810F-03E025079EB3}"/>
+    <hyperlink ref="K20" r:id="rId19" xr:uid="{EB5EBC38-48DF-47AA-89C5-E5147A2CCADD}"/>
+    <hyperlink ref="K21" r:id="rId20" xr:uid="{77802F46-9803-41E9-9477-705FD5AF7D30}"/>
+    <hyperlink ref="K22" r:id="rId21" xr:uid="{AD32246E-C00F-4FB6-93FB-7743ED98E74F}"/>
+    <hyperlink ref="K10" r:id="rId22" xr:uid="{A67F2EF4-4DF9-481B-BEAA-48016F302B1C}"/>
+    <hyperlink ref="C10" r:id="rId23" xr:uid="{77154953-0306-4761-8A48-36E76B504382}"/>
+    <hyperlink ref="K13:K14" r:id="rId24" display="aseguradosgw@gmail.com" xr:uid="{B64C1E98-F65B-4542-A589-503C52ABEEE9}"/>
+    <hyperlink ref="C14" r:id="rId25" xr:uid="{D9C14EFD-08B3-480C-A333-A20FA6DAB731}"/>
+    <hyperlink ref="C13" r:id="rId26" xr:uid="{945F7905-FC73-4F35-ABDE-B46FFD121B91}"/>
+    <hyperlink ref="K13" r:id="rId27" xr:uid="{A6FE7B60-6328-48B5-B33C-7C7AE0DF69EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualización data para generación regresión preprod
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroMotor.xlsx
+++ b/SuraClaims/GeneracionSiniestroMotor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759C3E0A-2114-48B5-A22C-233DEF9063C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57456016-6693-4A36-B0D0-034A020771A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="84">
   <si>
     <t>Usuario</t>
   </si>
@@ -267,10 +267,16 @@
     <t>04104019214</t>
   </si>
   <si>
-    <t>08/07/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04104017130 </t>
+    <t xml:space="preserve">04104017203 </t>
+  </si>
+  <si>
+    <t>14/07/2021</t>
+  </si>
+  <si>
+    <t>Robo Parcial (Otros)</t>
+  </si>
+  <si>
+    <t>Robo y/o Hurto Total Mano Armada</t>
   </si>
 </sst>
 </file>
@@ -365,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -386,6 +392,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -669,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,13 +1330,13 @@
         <v>21</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>42</v>
@@ -1359,13 +1366,13 @@
         <v>967</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S9" s="13" t="s">
         <v>9</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="U9" s="16"/>
       <c r="V9" s="13" t="s">
@@ -1380,7 +1387,7 @@
     </row>
     <row r="10" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>55</v>
@@ -1395,13 +1402,13 @@
         <v>21</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>42</v>
@@ -1431,13 +1438,16 @@
         <v>967</v>
       </c>
       <c r="R10" s="13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>31</v>
+        <v>41</v>
+      </c>
+      <c r="U10" s="13">
+        <v>23766</v>
       </c>
       <c r="V10" s="13" t="s">
         <v>8</v>
@@ -1451,7 +1461,7 @@
     </row>
     <row r="11" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>55</v>
@@ -1466,13 +1476,13 @@
         <v>21</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>42</v>
@@ -1502,34 +1512,28 @@
         <v>967</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="S11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="U11" s="16"/>
       <c r="V11" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="X11" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y11" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z11" s="13" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>55</v>
@@ -1544,13 +1548,13 @@
         <v>21</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>42</v>
@@ -1579,15 +1583,9 @@
       <c r="Q12" s="13">
         <v>967</v>
       </c>
-      <c r="R12" s="13" t="s">
-        <v>36</v>
-      </c>
       <c r="S12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="T12" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="V12" s="13" t="s">
         <v>9</v>
       </c>
@@ -1598,15 +1596,15 @@
         <v>8</v>
       </c>
       <c r="Y12" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z12" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="AA12" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>55</v>
@@ -1621,13 +1619,13 @@
         <v>21</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I13" s="17" t="s">
         <v>42</v>
@@ -1656,29 +1654,29 @@
       <c r="Q13" s="13">
         <v>967</v>
       </c>
-      <c r="R13" s="13" t="s">
-        <v>36</v>
-      </c>
       <c r="S13" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="T13" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="U13" s="16"/>
       <c r="V13" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="W13" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X13" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="Y13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z13" s="13" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>55</v>
@@ -1693,13 +1691,13 @@
         <v>21</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>42</v>
@@ -1729,13 +1727,10 @@
         <v>967</v>
       </c>
       <c r="R14" s="13" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="S14" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="T14" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="V14" s="13" t="s">
         <v>8</v>
@@ -1749,7 +1744,7 @@
     </row>
     <row r="15" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>55</v>
@@ -1764,13 +1759,13 @@
         <v>21</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I15" s="17" t="s">
         <v>42</v>
@@ -1799,28 +1794,22 @@
       <c r="Q15" s="13">
         <v>967</v>
       </c>
-      <c r="R15" s="13" t="s">
-        <v>36</v>
-      </c>
       <c r="S15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="T15" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="V15" s="13" t="s">
         <v>8</v>
       </c>
       <c r="W15" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X15" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>12</v>
+      <c r="A16" s="18">
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
@@ -1890,8 +1879,8 @@
       </c>
     </row>
     <row r="17" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>13</v>
+      <c r="A17" s="18">
+        <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>47</v>
@@ -1961,8 +1950,8 @@
       </c>
     </row>
     <row r="18" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>14</v>
+      <c r="A18" s="18">
+        <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>47</v>
@@ -2032,8 +2021,8 @@
       </c>
     </row>
     <row r="19" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>15</v>
+      <c r="A19" s="18">
+        <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>47</v>
@@ -2106,8 +2095,8 @@
       </c>
     </row>
     <row r="20" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>16</v>
+      <c r="A20" s="18">
+        <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>47</v>
@@ -2180,8 +2169,8 @@
       </c>
     </row>
     <row r="21" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>17</v>
+      <c r="A21" s="18">
+        <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>47</v>
@@ -2251,8 +2240,8 @@
       </c>
     </row>
     <row r="22" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>18</v>
+      <c r="A22" s="18">
+        <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>47</v>
@@ -2322,8 +2311,8 @@
       </c>
     </row>
     <row r="23" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>19</v>
+      <c r="A23" s="18">
+        <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>47</v>
@@ -2394,8 +2383,8 @@
       </c>
     </row>
     <row r="24" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>20</v>
+      <c r="A24" s="18">
+        <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>47</v>
@@ -2466,8 +2455,8 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>21</v>
+      <c r="A25" s="18">
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>47</v>
@@ -2540,8 +2529,8 @@
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>22</v>
+      <c r="A26" s="18">
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>47</v>
@@ -2614,8 +2603,8 @@
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>23</v>
+      <c r="A27" s="18">
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>

</xml_diff>